<commit_message>
Added headless flag, Test Summary and optimized Menu search flow
</commit_message>
<xml_diff>
--- a/Resources/ExcelTemplateForOutletCreation.xlsx
+++ b/Resources/ExcelTemplateForOutletCreation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="258">
   <si>
     <t>Outlet Code</t>
   </si>
@@ -433,6 +433,366 @@
   </si>
   <si>
     <t>03549211700</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLF6C52</t>
+  </si>
+  <si>
+    <t>03413148900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLDDED0</t>
+  </si>
+  <si>
+    <t>03414695300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLEEF25</t>
+  </si>
+  <si>
+    <t>03415590600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL4377C</t>
+  </si>
+  <si>
+    <t>03520723700</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL5FB76</t>
+  </si>
+  <si>
+    <t>03521739000</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL905DC</t>
+  </si>
+  <si>
+    <t>03522478200</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL1E1C6</t>
+  </si>
+  <si>
+    <t>03776234100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL4D284</t>
+  </si>
+  <si>
+    <t>03777302900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL59416</t>
+  </si>
+  <si>
+    <t>03778047800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLCB180</t>
+  </si>
+  <si>
+    <t>03478547800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL9B135</t>
+  </si>
+  <si>
+    <t>03479931200</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL1A3AF</t>
+  </si>
+  <si>
+    <t>03480851200</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLA2355</t>
+  </si>
+  <si>
+    <t>03531063600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL3F041</t>
+  </si>
+  <si>
+    <t>03531932100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL9A661</t>
+  </si>
+  <si>
+    <t>03532537700</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLFC4FF</t>
+  </si>
+  <si>
+    <t>03548174700</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLE399D</t>
+  </si>
+  <si>
+    <t>03549357400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL5924F</t>
+  </si>
+  <si>
+    <t>03550137100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLEBEF1</t>
+  </si>
+  <si>
+    <t>03971637300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL24B5F</t>
+  </si>
+  <si>
+    <t>03973677900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL96BAC</t>
+  </si>
+  <si>
+    <t>03974738400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLA8FDC</t>
+  </si>
+  <si>
+    <t>03807622800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLED6EB</t>
+  </si>
+  <si>
+    <t>03808988800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLAC781</t>
+  </si>
+  <si>
+    <t>03809881800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLA4236</t>
+  </si>
+  <si>
+    <t>03913833600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL703DB</t>
+  </si>
+  <si>
+    <t>03915067100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL2BD86</t>
+  </si>
+  <si>
+    <t>03915851800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL20E1D</t>
+  </si>
+  <si>
+    <t>03286627900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL7A851</t>
+  </si>
+  <si>
+    <t>03288901000</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL3722A</t>
+  </si>
+  <si>
+    <t>03290167300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLD42E5</t>
+  </si>
+  <si>
+    <t>03995745100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL5ECF0</t>
+  </si>
+  <si>
+    <t>03997402400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL84C1C</t>
+  </si>
+  <si>
+    <t>03998304800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLAD539</t>
+  </si>
+  <si>
+    <t>03091887900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL30FC2</t>
+  </si>
+  <si>
+    <t>03093059400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLF73DF</t>
+  </si>
+  <si>
+    <t>03093830700</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL35527</t>
+  </si>
+  <si>
+    <t>03118130500</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL64106</t>
+  </si>
+  <si>
+    <t>03119784300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLE8ABB</t>
+  </si>
+  <si>
+    <t>03120602800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL7B2B0</t>
+  </si>
+  <si>
+    <t>03912010500</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL6B102</t>
+  </si>
+  <si>
+    <t>03913307700</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLA6F81</t>
+  </si>
+  <si>
+    <t>03914669400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL65836</t>
+  </si>
+  <si>
+    <t>03285770200</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLE6617</t>
+  </si>
+  <si>
+    <t>03286792400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL1D653</t>
+  </si>
+  <si>
+    <t>03287389100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL92B67</t>
+  </si>
+  <si>
+    <t>03174403900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL3DD76</t>
+  </si>
+  <si>
+    <t>03175674900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL511B7</t>
+  </si>
+  <si>
+    <t>03176825600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLA9DA3</t>
+  </si>
+  <si>
+    <t>03142038900</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLE68D1</t>
+  </si>
+  <si>
+    <t>03143177300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL77D5A</t>
+  </si>
+  <si>
+    <t>03143957300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL1D8D0</t>
+  </si>
+  <si>
+    <t>03353459400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL5E531</t>
+  </si>
+  <si>
+    <t>03355129500</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLB9FAE</t>
+  </si>
+  <si>
+    <t>03355955600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL44C75</t>
+  </si>
+  <si>
+    <t>03824849500</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLE4FC9</t>
+  </si>
+  <si>
+    <t>03826570600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL186D0</t>
+  </si>
+  <si>
+    <t>03827758100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL24E5F</t>
+  </si>
+  <si>
+    <t>03539463400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLF9BA1</t>
+  </si>
+  <si>
+    <t>03540430200</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL8A7D9</t>
+  </si>
+  <si>
+    <t>03541077200</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1443,7 @@
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>95</v>
@@ -1113,7 +1473,7 @@
         <v>24.778867194283279</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>24.918102709670986</v>
+        <v>24.125126982276527</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>75</v>
@@ -1169,7 +1529,7 @@
       </c>
       <c r="AW2" s="5"/>
       <c r="AY2" s="12" t="s">
-        <v>133</v>
+        <v>253</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>88</v>
@@ -1207,7 +1567,7 @@
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>95</v>
@@ -1237,7 +1597,7 @@
         <v>24.473190244254056</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>24.10089653159682</v>
+        <v>24.349812618357568</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>75</v>
@@ -1293,7 +1653,7 @@
       </c>
       <c r="AW3" s="5"/>
       <c r="AY3" s="12" t="s">
-        <v>135</v>
+        <v>255</v>
       </c>
       <c r="AZ3" s="11" t="s">
         <v>88</v>
@@ -1331,7 +1691,7 @@
     </row>
     <row r="4" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>136</v>
+        <v>256</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>95</v>
@@ -1361,7 +1721,7 @@
         <v>24.955290746872056</v>
       </c>
       <c r="Q4" s="4" t="n">
-        <v>24.762808506327442</v>
+        <v>24.735438140229938</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>75</v>
@@ -1417,7 +1777,7 @@
       </c>
       <c r="AW4" s="5"/>
       <c r="AY4" s="12" t="s">
-        <v>137</v>
+        <v>257</v>
       </c>
       <c r="AZ4" s="11" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
Fixed multi user summary issue, fixed falkiness(added js click), made screenshot function and minor improvments
</commit_message>
<xml_diff>
--- a/Resources/ExcelTemplateForOutletCreation.xlsx
+++ b/Resources/ExcelTemplateForOutletCreation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="294">
   <si>
     <t>Outlet Code</t>
   </si>
@@ -865,6 +865,42 @@
   </si>
   <si>
     <t>03373138400</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLB37D4</t>
+  </si>
+  <si>
+    <t>03867266600</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLB321C</t>
+  </si>
+  <si>
+    <t>03869473800</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL25E02</t>
+  </si>
+  <si>
+    <t>03871485300</t>
+  </si>
+  <si>
+    <t>AUTO_OUTLF76E1</t>
+  </si>
+  <si>
+    <t>03973832500</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL5C0F0</t>
+  </si>
+  <si>
+    <t>03976278100</t>
+  </si>
+  <si>
+    <t>AUTO_OUTL721D0</t>
+  </si>
+  <si>
+    <t>03978246500</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1551,7 @@
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>95</v>
@@ -1545,7 +1581,7 @@
         <v>24.778867194283279</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>24.092802819185753</v>
+        <v>24.80217461268756</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>75</v>
@@ -1601,7 +1637,7 @@
       </c>
       <c r="AW2" s="5"/>
       <c r="AY2" s="12" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>88</v>
@@ -1639,7 +1675,7 @@
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>95</v>
@@ -1669,7 +1705,7 @@
         <v>24.473190244254056</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>24.602762606362692</v>
+        <v>24.661119311806317</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>75</v>
@@ -1725,7 +1761,7 @@
       </c>
       <c r="AW3" s="5"/>
       <c r="AY3" s="12" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="AZ3" s="11" t="s">
         <v>88</v>
@@ -1763,7 +1799,7 @@
     </row>
     <row r="4" spans="1:69" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>95</v>
@@ -1793,7 +1829,7 @@
         <v>24.955290746872056</v>
       </c>
       <c r="Q4" s="4" t="n">
-        <v>24.59323193727181</v>
+        <v>24.444845834022193</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>75</v>
@@ -1849,7 +1885,7 @@
       </c>
       <c r="AW4" s="5"/>
       <c r="AY4" s="12" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="AZ4" s="11" t="s">
         <v>88</v>

</xml_diff>